<commit_message>
Se cambian columnas en plantillas, se agregan rutas en appsetings para descarga de ciertas plantillas, filtrado de cabeceros
</commit_message>
<xml_diff>
--- a/WebAPI/wwwroot/Plantillas/ResumenCargaResultadosReglas.xlsx
+++ b/WebAPI/wwwroot/Plantillas/ResumenCargaResultadosReglas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nrojast\Documents\Plantillas_cu6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nayeli Rojas\Documents\SICA_INFOTEC\WebAPI\wwwroot\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="4296"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="4290"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -71,10 +71,10 @@
     <t>Cumple con todos los criterios para aplicar reglas?</t>
   </si>
   <si>
-    <t>Muestreo Validado por Irving</t>
-  </si>
-  <si>
     <t>% de pago</t>
+  </si>
+  <si>
+    <t>Muestreo Validado por</t>
   </si>
 </sst>
 </file>
@@ -418,16 +418,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="72" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,10 +472,10 @@
         <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>